<commit_message>
fixed add, delete, change. First sheet to upload
</commit_message>
<xml_diff>
--- a/data/map_data.xlsx
+++ b/data/map_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikdrean/Documents/python_projects/map_z_scraper/map_z_scraper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BF1DC8-B9EC-4647-8BD6-4D0CDD0AE76F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E673DA-F835-F246-B3B8-BDDE76FA665E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="24700" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="24680" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map_data_backup.csv" sheetId="1" r:id="rId1"/>
@@ -1001,16 +1001,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1037,9 +1030,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1342,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H166"/>
+  <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A164" sqref="A164:G164"/>
+      <selection activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4616,9 +4608,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="C166" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>